<commit_message>
Fixing typos in documentation
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobma\Documents\UIUC\CS 410 - Text Info Systems\Group Project\CourseProject\CourseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744D6B7D-6A9A-4329-A96D-0F62045FB794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B06BB5D-37E1-4DCA-B231-DBE6BAB12EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -113,10 +113,7 @@
     <t>Met with team, showed solution, worked with Cullen on how to set it up to work with his calling method, started documentation</t>
   </si>
   <si>
-    <t>Finishing documentation, video, arranging demo with reviewers</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>Finishing documentation, video, updating README, arranging demo with reviewers</t>
   </si>
 </sst>
 </file>
@@ -707,8 +704,8 @@
       <c r="A23" s="1">
         <v>44178</v>
       </c>
-      <c r="B23" t="s">
-        <v>26</v>
+      <c r="B23">
+        <v>2.75</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -717,7 +714,7 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>SUM(B2:B26)</f>
-        <v>33.25</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>

</xml_diff>